<commit_message>
validando roteiro, inserindo 'Ok' nas colunas
</commit_message>
<xml_diff>
--- a/QuartoPasso/finalizar reserva.xlsx
+++ b/QuartoPasso/finalizar reserva.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22223"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22229"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0F4D19C-077F-4610-94A1-4F2ED158C83E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A05EDEB3-6CE7-487C-B550-6AD206914C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,6 +139,9 @@
     <t>Quando o formulário não for válido o botão de finalizar reserva deve estar desabilitado</t>
   </si>
   <si>
+    <t>OK</t>
+  </si>
+  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -209,9 +212,6 @@
   </si>
   <si>
     <t>Ao apertar tab o foco está sendo alterado para o campo seguinte?</t>
-  </si>
-  <si>
-    <t>OK</t>
   </si>
   <si>
     <t>Após exibidas mensagens de erro a navegação está indo para a tela que contém o erro?</t>
@@ -1506,7 +1506,7 @@
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
     <cellStyle name="Texto Explicativo" xfId="2" builtinId="53" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="370">
+  <dxfs count="379">
     <dxf>
       <font>
         <b val="0"/>
@@ -3674,6 +3674,240 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFC3924"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFC3924"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99CC00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -11851,8 +12085,8 @@
   </sheetPr>
   <dimension ref="A2:AMK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -11935,7 +12169,7 @@
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>24</v>
@@ -11943,17 +12177,17 @@
     </row>
     <row r="7" spans="1:6" ht="45" outlineLevel="1">
       <c r="A7" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>24</v>
@@ -11961,17 +12195,17 @@
     </row>
     <row r="8" spans="1:6" ht="45" outlineLevel="1">
       <c r="A8" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>24</v>
@@ -11979,17 +12213,17 @@
     </row>
     <row r="9" spans="1:6" ht="30" outlineLevel="1">
       <c r="A9" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>24</v>
@@ -11997,17 +12231,17 @@
     </row>
     <row r="10" spans="1:6" ht="30" outlineLevel="1">
       <c r="A10" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="16" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>24</v>
@@ -12015,7 +12249,7 @@
     </row>
     <row r="11" spans="1:6" outlineLevel="1">
       <c r="A11" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -12029,7 +12263,7 @@
     </row>
     <row r="12" spans="1:6" outlineLevel="1">
       <c r="A12" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -12054,7 +12288,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="73" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="73"/>
       <c r="D14" s="11" t="s">
@@ -12087,7 +12321,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -12101,7 +12335,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -12115,7 +12349,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -12129,7 +12363,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -12143,7 +12377,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -12157,7 +12391,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -12171,7 +12405,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -12188,7 +12422,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="73" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="73"/>
       <c r="D24" s="11" t="s">
@@ -12221,7 +12455,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -12235,7 +12469,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -12249,7 +12483,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -12273,1041 +12507,1074 @@
     <mergeCell ref="E14:F14"/>
   </mergeCells>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="369" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="378" priority="29" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="368" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="30" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="367" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="376" priority="31" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4 E7:F7">
-    <cfRule type="cellIs" dxfId="366" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="375" priority="32" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="365" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="33" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="364" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="373" priority="34" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:F7">
-    <cfRule type="cellIs" dxfId="363" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="372" priority="35" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="362" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="36" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="361" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="370" priority="37" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:F7">
-    <cfRule type="cellIs" dxfId="360" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="369" priority="38" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="359" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="39" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="358" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="367" priority="40" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="cellIs" dxfId="357" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="366" priority="41" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="356" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="42" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="355" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="364" priority="43" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="cellIs" dxfId="354" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="363" priority="44" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="353" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="45" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="352" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="361" priority="46" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6:F7">
-    <cfRule type="cellIs" dxfId="351" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="360" priority="47" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="350" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="48" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="349" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="358" priority="49" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:F12">
-    <cfRule type="cellIs" dxfId="348" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="357" priority="50" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="347" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="51" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="346" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="355" priority="52" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:F12">
-    <cfRule type="cellIs" dxfId="345" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="354" priority="53" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="344" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="54" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="343" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="352" priority="55" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:F12">
-    <cfRule type="cellIs" dxfId="342" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="351" priority="56" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="341" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="57" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="340" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="349" priority="58" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="339" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="348" priority="59" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="338" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="60" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="337" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="346" priority="61" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="336" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="345" priority="62" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="335" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="63" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="334" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="343" priority="64" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="333" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="342" priority="65" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="332" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="66" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="331" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="340" priority="67" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="330" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="339" priority="68" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="329" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="69" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="328" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="337" priority="70" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="327" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="336" priority="71" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="326" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="72" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="325" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="334" priority="73" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="324" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="333" priority="74" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="323" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="75" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="322" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="331" priority="76" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:F11">
-    <cfRule type="cellIs" dxfId="321" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="330" priority="77" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="320" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="78" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="319" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="79" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:F11">
-    <cfRule type="cellIs" dxfId="318" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="327" priority="80" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="317" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="81" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="316" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="325" priority="82" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11:F11">
-    <cfRule type="cellIs" dxfId="315" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="83" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="314" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="84" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="313" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="322" priority="85" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:F11">
-    <cfRule type="cellIs" dxfId="312" priority="59" operator="equal">
+  <conditionalFormatting sqref="E11:F11 F10">
+    <cfRule type="cellIs" dxfId="321" priority="86" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="311" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="87" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="310" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="319" priority="88" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:F11">
-    <cfRule type="cellIs" dxfId="309" priority="62" operator="equal">
+  <conditionalFormatting sqref="E11:F11 F10">
+    <cfRule type="cellIs" dxfId="318" priority="89" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="308" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="90" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="307" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="316" priority="91" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:F11">
-    <cfRule type="cellIs" dxfId="306" priority="65" operator="equal">
+  <conditionalFormatting sqref="E11:F11 F10">
+    <cfRule type="cellIs" dxfId="315" priority="92" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="305" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="93" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="304" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="313" priority="94" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="cellIs" dxfId="312" priority="104" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="311" priority="105" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="310" priority="106" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="cellIs" dxfId="309" priority="107" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="308" priority="108" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="307" priority="109" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="cellIs" dxfId="306" priority="110" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="305" priority="111" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="304" priority="112" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="303" priority="113" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="302" priority="114" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="301" priority="115" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="300" priority="116" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="299" priority="117" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="298" priority="118" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="297" priority="119" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="296" priority="120" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="295" priority="121" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F9">
+    <cfRule type="cellIs" dxfId="294" priority="122" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="293" priority="123" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="292" priority="124" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F9">
+    <cfRule type="cellIs" dxfId="291" priority="125" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="290" priority="126" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="289" priority="127" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8:F9">
+    <cfRule type="cellIs" dxfId="288" priority="128" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="287" priority="129" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="286" priority="130" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="285" priority="140" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="284" priority="141" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="283" priority="142" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="282" priority="143" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="281" priority="144" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="280" priority="145" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="279" priority="146" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="278" priority="147" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="277" priority="148" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14 E17:F17">
+    <cfRule type="cellIs" dxfId="276" priority="149" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="275" priority="150" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="274" priority="151" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:F17">
+    <cfRule type="cellIs" dxfId="273" priority="152" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="272" priority="153" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="271" priority="154" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17:F17">
+    <cfRule type="cellIs" dxfId="270" priority="155" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="269" priority="156" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="268" priority="157" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:F17">
+    <cfRule type="cellIs" dxfId="267" priority="158" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="266" priority="159" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="265" priority="160" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:F17">
+    <cfRule type="cellIs" dxfId="264" priority="161" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="263" priority="162" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="262" priority="163" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16:F17">
+    <cfRule type="cellIs" dxfId="261" priority="164" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="260" priority="165" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="259" priority="166" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:F22">
+    <cfRule type="cellIs" dxfId="258" priority="167" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="257" priority="168" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="256" priority="169" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:F22">
+    <cfRule type="cellIs" dxfId="255" priority="170" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="254" priority="171" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="253" priority="172" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22:F22">
+    <cfRule type="cellIs" dxfId="252" priority="173" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="251" priority="174" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="250" priority="175" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="249" priority="176" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="248" priority="177" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="247" priority="178" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="246" priority="179" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="245" priority="180" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="244" priority="181" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="243" priority="182" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="242" priority="183" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="241" priority="184" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="240" priority="185" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="239" priority="186" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="238" priority="187" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="237" priority="188" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="236" priority="189" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="235" priority="190" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="234" priority="191" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="233" priority="192" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="232" priority="193" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21:F21">
+    <cfRule type="cellIs" dxfId="231" priority="194" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="230" priority="195" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="229" priority="196" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21:F21">
+    <cfRule type="cellIs" dxfId="228" priority="197" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="227" priority="198" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="226" priority="199" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21:F21">
+    <cfRule type="cellIs" dxfId="225" priority="200" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="224" priority="201" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="223" priority="202" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:F21">
+    <cfRule type="cellIs" dxfId="222" priority="203" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="221" priority="204" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="220" priority="205" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:F21">
+    <cfRule type="cellIs" dxfId="219" priority="206" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="218" priority="207" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="217" priority="208" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:F21">
+    <cfRule type="cellIs" dxfId="216" priority="209" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="215" priority="210" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="214" priority="211" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="213" priority="212" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="212" priority="213" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="211" priority="214" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="210" priority="215" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="209" priority="216" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="208" priority="217" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="207" priority="218" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="219" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="205" priority="220" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="cellIs" dxfId="204" priority="221" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="203" priority="222" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="202" priority="223" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="cellIs" dxfId="201" priority="224" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="200" priority="225" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="199" priority="226" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="cellIs" dxfId="198" priority="227" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="197" priority="228" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="196" priority="229" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19:F19">
+    <cfRule type="cellIs" dxfId="195" priority="230" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="194" priority="231" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="193" priority="232" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19:F19">
+    <cfRule type="cellIs" dxfId="192" priority="233" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="191" priority="234" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="190" priority="235" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19:F19">
+    <cfRule type="cellIs" dxfId="189" priority="236" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="188" priority="237" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="187" priority="238" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:F19">
+    <cfRule type="cellIs" dxfId="186" priority="239" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="185" priority="240" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="184" priority="241" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:F19">
+    <cfRule type="cellIs" dxfId="183" priority="242" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="182" priority="243" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="181" priority="244" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:F19">
+    <cfRule type="cellIs" dxfId="180" priority="245" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="246" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="178" priority="247" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" dxfId="177" priority="248" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="249" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="175" priority="250" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" dxfId="174" priority="251" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="173" priority="252" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="253" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" dxfId="171" priority="254" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="255" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="169" priority="256" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="168" priority="257" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="167" priority="258" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="259" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="165" priority="260" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="261" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="163" priority="262" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="162" priority="263" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="161" priority="264" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="265" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24 E27:F27">
+    <cfRule type="cellIs" dxfId="159" priority="266" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="267" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="268" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:F27">
+    <cfRule type="cellIs" dxfId="156" priority="269" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="155" priority="270" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="271" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:F27">
+    <cfRule type="cellIs" dxfId="153" priority="272" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="273" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="274" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:F27">
+    <cfRule type="cellIs" dxfId="150" priority="275" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="276" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="277" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:F27">
+    <cfRule type="cellIs" dxfId="147" priority="278" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="279" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="280" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26:F27">
+    <cfRule type="cellIs" dxfId="144" priority="281" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="282" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="283" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:F28">
+    <cfRule type="cellIs" dxfId="141" priority="284" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="285" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="286" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:F28">
+    <cfRule type="cellIs" dxfId="138" priority="287" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="288" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="289" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28:F28">
+    <cfRule type="cellIs" dxfId="135" priority="290" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="291" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="292" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="cellIs" dxfId="132" priority="293" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="294" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="295" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="cellIs" dxfId="129" priority="296" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="297" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="298" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="cellIs" dxfId="126" priority="299" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="300" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="301" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="cellIs" dxfId="123" priority="302" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="303" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="304" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="cellIs" dxfId="120" priority="305" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="306" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="307" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28">
+    <cfRule type="cellIs" dxfId="117" priority="308" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="309" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="310" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="114" priority="19" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="20" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="21" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="111" priority="22" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="23" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="109" priority="24" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="108" priority="25" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="26" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="27" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="105" priority="10" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="11" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="12" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="102" priority="13" operator="equal">
+      <formula>"Concluído"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="14" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="15" operator="equal">
+      <formula>"Aguardando Teste"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="99" priority="16" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="17" operator="equal">
+      <formula>"Erro"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="18" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="303" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="302" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="2" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="301" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="3" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="300" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="4" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="299" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="5" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="298" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="6" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="297" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="7" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="296" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="8" operator="equal">
       <formula>"Erro"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="295" priority="76" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="294" priority="77" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="293" priority="78" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="292" priority="79" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="291" priority="80" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="290" priority="81" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="289" priority="82" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="288" priority="83" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="287" priority="84" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="286" priority="85" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:F9">
-    <cfRule type="cellIs" dxfId="285" priority="86" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="284" priority="87" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="283" priority="88" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:F9">
-    <cfRule type="cellIs" dxfId="282" priority="89" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="90" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="280" priority="91" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:F9">
-    <cfRule type="cellIs" dxfId="279" priority="92" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="278" priority="93" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="277" priority="94" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8:F9">
-    <cfRule type="cellIs" dxfId="276" priority="95" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="275" priority="96" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="274" priority="97" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8:F9">
-    <cfRule type="cellIs" dxfId="273" priority="98" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="272" priority="99" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="271" priority="100" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8:F9">
-    <cfRule type="cellIs" dxfId="270" priority="101" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="269" priority="102" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="268" priority="103" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="267" priority="104" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="266" priority="105" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="265" priority="106" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="264" priority="107" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="263" priority="108" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="262" priority="109" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="261" priority="110" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="260" priority="111" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="259" priority="112" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="258" priority="113" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="114" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="256" priority="115" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="255" priority="116" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="254" priority="117" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="253" priority="118" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="252" priority="119" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="120" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="250" priority="121" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14 E17:F17">
-    <cfRule type="cellIs" dxfId="249" priority="122" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="248" priority="123" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="247" priority="124" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17:F17">
-    <cfRule type="cellIs" dxfId="246" priority="125" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="245" priority="126" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="244" priority="127" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17:F17">
-    <cfRule type="cellIs" dxfId="243" priority="128" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="129" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="241" priority="130" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16:F17">
-    <cfRule type="cellIs" dxfId="240" priority="131" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="132" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="238" priority="133" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16:F17">
-    <cfRule type="cellIs" dxfId="237" priority="134" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="135" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="235" priority="136" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16:F17">
-    <cfRule type="cellIs" dxfId="234" priority="137" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="138" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="232" priority="139" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:F22">
-    <cfRule type="cellIs" dxfId="231" priority="140" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="230" priority="141" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="229" priority="142" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:F22">
-    <cfRule type="cellIs" dxfId="228" priority="143" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="144" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="226" priority="145" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22:F22">
-    <cfRule type="cellIs" dxfId="225" priority="146" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="147" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="223" priority="148" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="222" priority="149" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="150" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="220" priority="151" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="219" priority="152" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="153" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="217" priority="154" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="216" priority="155" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="156" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="157" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="213" priority="158" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="159" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="160" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="210" priority="161" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="162" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="208" priority="163" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="207" priority="164" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="165" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="205" priority="166" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21:F21">
-    <cfRule type="cellIs" dxfId="204" priority="167" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="168" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="169" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21:F21">
-    <cfRule type="cellIs" dxfId="201" priority="170" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="171" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="199" priority="172" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21:F21">
-    <cfRule type="cellIs" dxfId="198" priority="173" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="174" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="175" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20:F21">
-    <cfRule type="cellIs" dxfId="195" priority="176" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="177" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="178" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20:F21">
-    <cfRule type="cellIs" dxfId="192" priority="179" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="180" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="181" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20:F21">
-    <cfRule type="cellIs" dxfId="189" priority="182" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="183" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="184" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="186" priority="185" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="186" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="187" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="183" priority="188" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="189" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="190" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="180" priority="191" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="192" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="193" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="177" priority="194" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="195" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="196" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="174" priority="197" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="198" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="199" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="171" priority="200" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="201" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="202" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19:F19">
-    <cfRule type="cellIs" dxfId="168" priority="203" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="204" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="205" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19:F19">
-    <cfRule type="cellIs" dxfId="165" priority="206" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="207" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="208" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19:F19">
-    <cfRule type="cellIs" dxfId="162" priority="209" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="210" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="211" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:F19">
-    <cfRule type="cellIs" dxfId="159" priority="212" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="213" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="214" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:F19">
-    <cfRule type="cellIs" dxfId="156" priority="215" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="216" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="217" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:F19">
-    <cfRule type="cellIs" dxfId="153" priority="218" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="219" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="220" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="150" priority="221" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="222" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="223" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="147" priority="224" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="225" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="226" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="144" priority="227" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="228" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="229" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="141" priority="230" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="231" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="232" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="138" priority="233" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="234" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="235" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="135" priority="236" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="237" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="238" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24 E27:F27">
-    <cfRule type="cellIs" dxfId="132" priority="239" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="240" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="241" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27:F27">
-    <cfRule type="cellIs" dxfId="129" priority="242" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="243" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="244" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27:F27">
-    <cfRule type="cellIs" dxfId="126" priority="245" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="246" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="247" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:F27">
-    <cfRule type="cellIs" dxfId="123" priority="248" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="249" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="250" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:F27">
-    <cfRule type="cellIs" dxfId="120" priority="251" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="252" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="253" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:F27">
-    <cfRule type="cellIs" dxfId="117" priority="254" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="255" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="256" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28:F28">
-    <cfRule type="cellIs" dxfId="114" priority="257" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="258" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="259" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28:F28">
-    <cfRule type="cellIs" dxfId="111" priority="260" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="261" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="262" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28:F28">
-    <cfRule type="cellIs" dxfId="108" priority="263" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="264" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="265" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="105" priority="266" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="267" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="268" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="102" priority="269" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="270" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="271" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="99" priority="272" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="273" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="274" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="96" priority="275" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="276" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="277" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="93" priority="278" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="279" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="280" operator="equal">
-      <formula>"Aguardando Teste"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F28">
-    <cfRule type="cellIs" dxfId="90" priority="281" operator="equal">
-      <formula>"OK"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="282" operator="equal">
-      <formula>"Erro"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="283" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="9" operator="equal">
       <formula>"Aguardando Teste"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:F12 E16:F22 E26:F28" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26:F28 E16:F22 E6:F12" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Aguardando Teste,OK,Erro,NA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -13347,20 +13614,20 @@
     <row r="1" spans="2:4" s="2" customFormat="1"/>
     <row r="2" spans="2:4" ht="18" customHeight="1">
       <c r="B2" s="72" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
     </row>
     <row r="3" spans="2:4" ht="13.9" customHeight="1">
       <c r="B3" s="79" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="13.9">
@@ -14843,15 +15110,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BB46273AC895BC429CDD381D3691D2B9" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="e1ce5b6e83737eb8f009b640c30fa88d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="35aeef18-1e63-474b-8ce4-f5abefe28d84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dc4da7a948ec9821969ad36af22710a" ns2:_="">
     <xsd:import namespace="35aeef18-1e63-474b-8ce4-f5abefe28d84"/>
@@ -14983,14 +15241,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B853C070-DD64-4DFA-A826-7E95875889C8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A700B593-5E25-4ABB-A05F-A033C4E38350}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B5FDA3F-AA6B-418A-B72B-3C3F360D3D08}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B5FDA3F-AA6B-418A-B72B-3C3F360D3D08}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A700B593-5E25-4ABB-A05F-A033C4E38350}"/>
 </file>
</xml_diff>